<commit_message>
Complete references; fix Green Corridor photo; add Kent Ridge map
</commit_message>
<xml_diff>
--- a/assets/Sources.xlsx
+++ b/assets/Sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Christian\Box\data&amp;stuff\aces-active.github.io\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58215321-FAC6-4F6A-BE51-B7DD63DC484F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B33F83F-CE82-470D-B017-51FD4B5385AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28965" yWindow="-435" windowWidth="15900" windowHeight="11295" activeTab="1" xr2:uid="{08BF9BF0-21A4-4DD6-AFBD-CD3E0D1D4E78}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="139">
   <si>
     <t>Image</t>
   </si>
@@ -450,6 +450,9 @@
   </si>
   <si>
     <t>Facebook</t>
+  </si>
+  <si>
+    <t>MyWoWo</t>
   </si>
 </sst>
 </file>
@@ -1842,8 +1845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0AC244B-463F-4A70-A609-63E8A7E6DE82}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2548,7 +2551,7 @@
         <v>106</v>
       </c>
       <c r="D44" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>